<commit_message>
Delete exam and batch info done!
</commit_message>
<xml_diff>
--- a/lib/uploads/2017_1_A_PT-1.xlsx
+++ b/lib/uploads/2017_1_A_PT-1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>GYAN GANGA INTERNATIONAL SCHOOL</t>
   </si>
@@ -56,6 +56,24 @@
   </si>
   <si>
     <t>PERIODIC TEST-1 (PT-1)</t>
+  </si>
+  <si>
+    <t>Deb</t>
+  </si>
+  <si>
+    <t>Gupta</t>
+  </si>
+  <si>
+    <t>Sharma</t>
+  </si>
+  <si>
+    <t>Legen-wait for it-dary</t>
+  </si>
+  <si>
+    <t>Pathetic</t>
+  </si>
+  <si>
+    <t>Awesome</t>
   </si>
 </sst>
 </file>
@@ -787,7 +805,7 @@
   <dimension ref="A1:R56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -941,8 +959,12 @@
       <c r="G7" s="16">
         <v>20</v>
       </c>
-      <c r="H7" s="28"/>
-      <c r="I7" s="29"/>
+      <c r="H7" s="28">
+        <v>70</v>
+      </c>
+      <c r="I7" s="29">
+        <v>50</v>
+      </c>
       <c r="J7" s="30"/>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
@@ -957,15 +979,34 @@
       <c r="A8" s="3">
         <v>1</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="3"/>
+      <c r="B8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="3">
+        <v>19</v>
+      </c>
+      <c r="D8" s="3">
+        <v>5</v>
+      </c>
+      <c r="E8" s="3">
+        <v>6</v>
+      </c>
+      <c r="F8" s="3">
+        <v>10</v>
+      </c>
+      <c r="G8" s="4">
+        <v>15</v>
+      </c>
+      <c r="H8" s="26">
+        <f>C8+D8+E8+F8+G8</f>
+        <v>55</v>
+      </c>
+      <c r="I8" s="27">
+        <v>25</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
       <c r="M8" s="7"/>
@@ -979,15 +1020,34 @@
       <c r="A9" s="2">
         <v>2</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="2">
+        <v>15</v>
+      </c>
+      <c r="D9" s="2">
+        <v>5</v>
+      </c>
+      <c r="E9" s="2">
+        <v>10</v>
+      </c>
+      <c r="F9" s="2">
+        <v>9</v>
+      </c>
+      <c r="G9" s="5">
+        <v>14</v>
+      </c>
+      <c r="H9" s="26">
+        <f t="shared" ref="H9:H10" si="0">C9+D9+E9+F9+G9</f>
+        <v>53</v>
+      </c>
+      <c r="I9" s="13">
+        <v>48</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
@@ -1001,15 +1061,34 @@
       <c r="A10" s="2">
         <v>3</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="2"/>
+      <c r="B10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="2">
+        <v>13</v>
+      </c>
+      <c r="D10" s="2">
+        <v>7</v>
+      </c>
+      <c r="E10" s="2">
+        <v>9</v>
+      </c>
+      <c r="F10" s="2">
+        <v>8</v>
+      </c>
+      <c r="G10" s="5">
+        <v>18</v>
+      </c>
+      <c r="H10" s="26">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="I10" s="13">
+        <v>50</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
@@ -1020,9 +1099,7 @@
       <c r="R10" s="7"/>
     </row>
     <row r="11" spans="1:18">
-      <c r="A11" s="3">
-        <v>4</v>
-      </c>
+      <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -1042,9 +1119,7 @@
       <c r="R11" s="7"/>
     </row>
     <row r="12" spans="1:18">
-      <c r="A12" s="2">
-        <v>5</v>
-      </c>
+      <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -1064,9 +1139,7 @@
       <c r="R12" s="7"/>
     </row>
     <row r="13" spans="1:18">
-      <c r="A13" s="2">
-        <v>6</v>
-      </c>
+      <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -1086,9 +1159,7 @@
       <c r="R13" s="7"/>
     </row>
     <row r="14" spans="1:18">
-      <c r="A14" s="3">
-        <v>7</v>
-      </c>
+      <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -1108,9 +1179,7 @@
       <c r="R14" s="7"/>
     </row>
     <row r="15" spans="1:18">
-      <c r="A15" s="2">
-        <v>8</v>
-      </c>
+      <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -1130,9 +1199,7 @@
       <c r="R15" s="7"/>
     </row>
     <row r="16" spans="1:18">
-      <c r="A16" s="2">
-        <v>9</v>
-      </c>
+      <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -1152,9 +1219,7 @@
       <c r="R16" s="7"/>
     </row>
     <row r="17" spans="1:18">
-      <c r="A17" s="3">
-        <v>10</v>
-      </c>
+      <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -1174,9 +1239,7 @@
       <c r="R17" s="7"/>
     </row>
     <row r="18" spans="1:18">
-      <c r="A18" s="2">
-        <v>11</v>
-      </c>
+      <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -1196,9 +1259,7 @@
       <c r="R18" s="7"/>
     </row>
     <row r="19" spans="1:18">
-      <c r="A19" s="2">
-        <v>12</v>
-      </c>
+      <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -1218,9 +1279,7 @@
       <c r="R19" s="7"/>
     </row>
     <row r="20" spans="1:18">
-      <c r="A20" s="3">
-        <v>13</v>
-      </c>
+      <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>

</xml_diff>